<commit_message>
201904121740 on cleaning data more accurately
</commit_message>
<xml_diff>
--- a/data/leave_and_attend_legislators.xlsx
+++ b/data/leave_and_attend_legislators.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\scripts\R\vote_record\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\scripts\R\vote_record\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE070FD-81A0-4D0B-B2C9-01E6F78C3FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leave_and_attend_legislators" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>legislator_name</t>
   </si>
@@ -258,12 +259,25 @@
   </si>
   <si>
     <t>Kolas Yotaka　　周春米</t>
+  </si>
+  <si>
+    <t>Kolas
+Yotaka吳秉叡</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/03/08/LCEWC03_090308.htm</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>106/04/07, 106/04/11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -850,12 +864,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1177,12 +1194,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1781,8 +1803,38 @@
         <v>78</v>
       </c>
     </row>
+    <row r="22" spans="1:9" ht="33" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="2">
+        <v>58</v>
+      </c>
+      <c r="H22" t="s">
+        <v>81</v>
+      </c>
+      <c r="I22" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
201905052230 modified a lot 政黨壓力指標 and LCA and debug for duplicated 限制版資料 dataset and prepare for package clustering computation(using AWS) and survey(weighted)
</commit_message>
<xml_diff>
--- a/data/leave_and_attend_legislators.xlsx
+++ b/data/leave_and_attend_legislators.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software\scripts\R\vote_record\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r03a21033\Downloads\vote_record\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE070FD-81A0-4D0B-B2C9-01E6F78C3FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="leave_and_attend_legislators" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>legislator_name</t>
   </si>
@@ -37,153 +36,66 @@
     <t>meetingno</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>urln</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>replace_with</t>
   </si>
   <si>
     <t>委員出席　210人　</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec/02/06/01/09/LCEWC03_060109.htm</t>
-  </si>
-  <si>
-    <t>094/04/22, 094/04/26</t>
-  </si>
-  <si>
     <t>委員出席　112人　</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec/02/07/01/16/LCEWC03_070116.htm</t>
-  </si>
-  <si>
-    <t>097/06/19, 097/06/20, 097/06/24</t>
-  </si>
-  <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec/02/07/03/13/LCEWC03_070313.htm</t>
-  </si>
-  <si>
-    <t>098/05/15, 098/05/19</t>
-  </si>
-  <si>
     <t>翁重鈞　高志鵬</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec/02/07/05/05/LCEWC03_070505.htm</t>
-  </si>
-  <si>
-    <t>099/03/19, 099/03/23</t>
-  </si>
-  <si>
     <t>翁重鈞　　高志鵬</t>
   </si>
   <si>
     <t>邱　毅 　楊仁福</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec/02/07/08/06/LCEWC03_070806.htm</t>
-  </si>
-  <si>
-    <t>100/10/21, 100/10/25</t>
-  </si>
-  <si>
     <t>邱　毅 　　楊仁福</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/08/02/11/LCEWC03_080211.htm</t>
-  </si>
-  <si>
-    <t>101/11/30, 101/12/04</t>
-  </si>
-  <si>
     <t>鄭天財(Sra．Kacaw)　葉津鈴</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/08/06/02/LCEWC03_080602.htm</t>
-  </si>
-  <si>
-    <t>103/09/19, 103/09/23</t>
-  </si>
-  <si>
     <t>鄭天財　　葉津鈴</t>
   </si>
   <si>
     <t>鄭天財(Sra．Kacaw)　李貴敏</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/08/06/07/LCEWC03_080607.htm</t>
-  </si>
-  <si>
-    <t>103/10/24, 103/10/28</t>
-  </si>
-  <si>
     <t>鄭天財　　李貴敏</t>
   </si>
   <si>
     <t>鄭天財Sra．Kacaw 陳鎮湘</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/08/08/02/LCEWC03_080802.htm</t>
-  </si>
-  <si>
-    <t>104/09/18, 104/09/21, 104/09/22</t>
-  </si>
-  <si>
     <t>鄭天財　　陳鎮湘</t>
   </si>
   <si>
     <t>蔡易餘　林岱樺</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/01/04/LCEWC03_090104.htm</t>
-  </si>
-  <si>
-    <t>105/03/11, 105/03/15</t>
-  </si>
-  <si>
     <t>蔡易餘　　林岱樺</t>
   </si>
   <si>
     <t>Kolas Yotaka陳素月</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/02/01/LCEWC03_090201.htm</t>
-  </si>
-  <si>
-    <t>105/09/13</t>
-  </si>
-  <si>
     <t>Kolas Yotaka　　陳素月</t>
   </si>
   <si>
     <t>徐國勇（9月30日） 江永昌</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/02/04/LCEWC03_090204.htm</t>
-  </si>
-  <si>
-    <t>105/09/30, 105/10/03, 105/10/04</t>
-  </si>
-  <si>
     <t>徐國勇　　江永昌</t>
   </si>
   <si>
     <t>廖國棟Sufin．Siluko 黃昭順</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/02/17/LCEWC03_090217.htm</t>
-  </si>
-  <si>
-    <t>105/12/30</t>
-  </si>
-  <si>
     <t>廖國棟Sufin．Siluko　　黃昭順</t>
   </si>
   <si>
@@ -196,22 +108,10 @@
     <t>Kolas Yotaka葉宜津</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/03/09/02/01/01/LCEWC03_09020101.htm</t>
-  </si>
-  <si>
-    <t>106/01/05, 106/01/06, 106/01/10, 106/01/11, 106/01/12</t>
-  </si>
-  <si>
     <t>Kolas Yotaka　　葉宜津</t>
   </si>
   <si>
     <t>Kolas Yotaka蕭美琴</t>
-  </si>
-  <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/03/04/LCEWC03_090304.htm</t>
-  </si>
-  <si>
-    <t>106/03/10, 106/03/14</t>
   </si>
   <si>
     <t>Kolas Yotaka　　蕭美琴</t>
@@ -224,38 +124,16 @@
     <t>高潞．以用．巴魕剌Kawlo．Iyun．Pacidal　　陳其邁</t>
   </si>
   <si>
-    <t>Kolas_x000D_
-Yotaka吳秉叡</t>
-  </si>
-  <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/03/08/LCEWC03_090308.htm</t>
-  </si>
-  <si>
-    <t>106/04/07, 106/04/11</t>
-  </si>
-  <si>
     <t>Kolas Yotaka　　吳秉叡</t>
   </si>
   <si>
     <t>廖國棟Sufin．Siluko 徐榛蔚</t>
   </si>
   <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/03/09/03/03/01/LCEWC03_09030301.htm</t>
-  </si>
-  <si>
-    <t>106/08/18, 106/08/21</t>
-  </si>
-  <si>
     <t>廖國棟Sufin．Siluko　　徐榛蔚</t>
   </si>
   <si>
     <t>Kolas Yotaka周春米</t>
-  </si>
-  <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/04/11/LCEWC03_090411.htm</t>
-  </si>
-  <si>
-    <t>106/12/01, 106/12/05</t>
   </si>
   <si>
     <t>Kolas Yotaka　　周春米</t>
@@ -263,21 +141,13 @@
   <si>
     <t>Kolas
 Yotaka吳秉叡</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://lci.ly.gov.tw/LyLCEW/html/agendarec1/02/09/03/08/LCEWC03_090308.htm</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>106/04/07, 106/04/11</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -864,15 +734,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1194,11 +1061,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1073,7 @@
     <col min="1" max="1" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1225,19 +1092,10 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2">
         <v>6</v>
@@ -1251,19 +1109,10 @@
       <c r="E2">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>7</v>
@@ -1277,19 +1126,10 @@
       <c r="E3">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
-        <v>111</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -1303,19 +1143,10 @@
       <c r="E4">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>127</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -1330,21 +1161,12 @@
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5">
-        <v>199</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>7</v>
@@ -1359,21 +1181,12 @@
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6">
-        <v>250</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -1387,19 +1200,10 @@
       <c r="E7">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7">
-        <v>262</v>
-      </c>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>8</v>
@@ -1414,21 +1218,12 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8">
-        <v>336</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1443,21 +1238,12 @@
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9">
-        <v>331</v>
-      </c>
-      <c r="H9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -1472,21 +1258,12 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10">
-        <v>400</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="B11">
         <v>9</v>
@@ -1501,21 +1278,12 @@
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11">
-        <v>384</v>
-      </c>
-      <c r="H11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -1530,21 +1298,12 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12">
-        <v>414</v>
-      </c>
-      <c r="H12" t="s">
-        <v>45</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -1559,21 +1318,12 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13">
-        <v>411</v>
-      </c>
-      <c r="H13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -1588,21 +1338,12 @@
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14">
-        <v>448</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>9</v>
@@ -1617,21 +1358,12 @@
         <v>17</v>
       </c>
       <c r="F15" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15">
-        <v>448</v>
-      </c>
-      <c r="H15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -1646,21 +1378,12 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16">
-        <v>447</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1675,21 +1398,12 @@
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17">
-        <v>440</v>
-      </c>
-      <c r="H17" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="99" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1704,21 +1418,12 @@
         <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18">
-        <v>440</v>
-      </c>
-      <c r="H18" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="49.5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="33" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -1733,21 +1438,12 @@
         <v>8</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19">
-        <v>436</v>
-      </c>
-      <c r="H19" t="s">
-        <v>69</v>
-      </c>
-      <c r="I19" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -1762,21 +1458,12 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20">
-        <v>470</v>
-      </c>
-      <c r="H20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>9</v>
@@ -1791,48 +1478,16 @@
         <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21">
-        <v>457</v>
-      </c>
-      <c r="H21" t="s">
-        <v>77</v>
-      </c>
-      <c r="I21" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="33" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B22">
-        <v>9</v>
-      </c>
-      <c r="C22">
-        <v>3</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>8</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G22" s="2">
-        <v>58</v>
-      </c>
-      <c r="H22" t="s">
-        <v>81</v>
-      </c>
-      <c r="I22" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I21">
+    <sortCondition ref="B2:B21"/>
+    <sortCondition ref="C2:C21"/>
+    <sortCondition ref="D2:D21"/>
+    <sortCondition ref="E2:E21"/>
+  </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>